<commit_message>
add entity management test cases, 3rd batch
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBC1C96-683C-4E1B-9C0F-20C263517011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C2A010-CB1D-4BA1-A04B-CC518903B2E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="createEntityInDomain" sheetId="5" r:id="rId1"/>
     <sheet name="updateEntity" sheetId="3" r:id="rId2"/>
     <sheet name="deleteEntity" sheetId="4" r:id="rId3"/>
     <sheet name="getEntityById" sheetId="2" r:id="rId4"/>
+    <sheet name="getRelations" sheetId="6" r:id="rId5"/>
+    <sheet name="getRelationById" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
   <si>
     <t>OK</t>
   </si>
@@ -163,6 +165,69 @@
   </si>
   <si>
     <t>SNC-Entity-mgmt-Test-5-var1</t>
+  </si>
+  <si>
+    <t>labels</t>
+  </si>
+  <si>
+    <t>SNC-Entity-mgmt-Test-17-var1</t>
+  </si>
+  <si>
+    <t>produced</t>
+  </si>
+  <si>
+    <t>produced, has</t>
+  </si>
+  <si>
+    <t>bad request, label not exist</t>
+  </si>
+  <si>
+    <t>SNC-Entity-mgmt-Test-17-var2</t>
+  </si>
+  <si>
+    <t>SNC-Entity-mgmt-Test-17-var3</t>
+  </si>
+  <si>
+    <t>SNC-Entity-mgmt-Test-17-var4</t>
+  </si>
+  <si>
+    <t>good request, single valid label</t>
+  </si>
+  <si>
+    <t>good request, multiple valid labels</t>
+  </si>
+  <si>
+    <t>not_exist_relation</t>
+  </si>
+  <si>
+    <t>produced, not_exist_relation</t>
+  </si>
+  <si>
+    <t>good request, get all relations</t>
+  </si>
+  <si>
+    <t>SNC-Entity-mgmt-Test-17-var5</t>
+  </si>
+  <si>
+    <t>good request, mix of valid and invalid labels</t>
+  </si>
+  <si>
+    <t>relationId</t>
+  </si>
+  <si>
+    <t>SNC-Entity-mgmt-Test-18</t>
+  </si>
+  <si>
+    <t>bad request</t>
+  </si>
+  <si>
+    <t>getRelationById.relationId: id format invalid</t>
+  </si>
+  <si>
+    <t>SNC-Entity-mgmt-Test-19-var1</t>
+  </si>
+  <si>
+    <t>SNC-Entity-mgmt-Test-19-var2</t>
   </si>
 </sst>
 </file>
@@ -191,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -241,6 +312,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68ECACFD-75AA-40A8-8500-FACA5E36F33B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1012,4 +1084,248 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7825D-C3D3-4455-B765-0D831E376750}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6328125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="12.54296875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6">
+        <v>200</v>
+      </c>
+      <c r="E2" s="6">
+        <v>200</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="2">
+        <v>200</v>
+      </c>
+      <c r="E3" s="2">
+        <v>200</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="2">
+        <v>200</v>
+      </c>
+      <c r="E4" s="2">
+        <v>200</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="2">
+        <v>200</v>
+      </c>
+      <c r="E5" s="2">
+        <v>200</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2">
+        <v>200</v>
+      </c>
+      <c r="E6" s="2">
+        <v>200</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8CB3E4-B830-482F-A87D-FE5107D53FAD}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="12.54296875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6">
+        <v>265</v>
+      </c>
+      <c r="D2" s="6">
+        <v>200</v>
+      </c>
+      <c r="E2" s="6">
+        <v>200</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>400</v>
+      </c>
+      <c r="E3" s="2">
+        <v>103000</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2">
+        <v>9999</v>
+      </c>
+      <c r="D4" s="2">
+        <v>500</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updte snc-entityMgmt-deleteRelations-Test-1 and 2
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D131EE45-D5CA-4117-8924-42D92C317B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C1C2AE-A808-4479-8AB6-2B1F7D3864AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="createEntities" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="141">
   <si>
     <t>testEntity1</t>
   </si>
@@ -414,25 +414,6 @@
     <t>1234,5678</t>
   </si>
   <si>
-    <t>[
-  {
-    "id" : "1234",
-    "label" : "testEntity1ForRelation",
-    "properties" : {
-      "metadata_node_type" : "entity"
-    }
-  },
-  {
-    "id" : "1234",
-    "label" : "testEntity2ForRelation",
-    "properties" : {
-    "metadata_node_type" : "instance",
-    "metadata_node_pk":"id"
-    }
-  }
-]</t>
-  </si>
-  <si>
     <t>good request,create one relation,data received</t>
   </si>
   <si>
@@ -490,9 +471,6 @@
     <t>pre-executionOfCreateEntities</t>
   </si>
   <si>
-    <t>good request,update multiple relations,data received</t>
-  </si>
-  <si>
     <t>snc-entityMgmt-getRelationById-Test-1</t>
   </si>
   <si>
@@ -535,13 +513,7 @@
     <t>good request,delete one relation</t>
   </si>
   <si>
-    <t>testRelation1,testRelation2</t>
-  </si>
-  <si>
     <t>snc-entityMgmt-deleteRelations-Test-4</t>
-  </si>
-  <si>
-    <t>good request,delete multiple relations</t>
   </si>
   <si>
     <t>[
@@ -662,6 +634,15 @@
 ]</t>
   </si>
   <si>
+    <t>not exists</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>101400</t>
+  </si>
+  <si>
     <t>[
   {
     "id": "1234",
@@ -671,9 +652,11 @@
       "relation": "one-to-one",
       "typevalue": "id:id"
     },
-    "out": "$entity1ForRelation"
+    "out": "$entity1ForRelation",
+    "in": "$entity2ForRelation"
   }
 ]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>[
@@ -700,6 +683,42 @@
     "in": "$entity2ForRelation"
   }
 ]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[
+  {
+    "id" : "1234",
+    "label" : "entity1ForRelation",
+    "properties" : {
+      "metadata_node_type" : "entity"
+    }
+  },
+  {
+    "id" : "1234",
+    "label" : "entity2ForRelation",
+    "properties" : {
+    "metadata_node_type" : "instance",
+    "metadata_node_pk":"id"
+    }
+  }
+]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[
+  {
+    "id": "1234",
+    "label": "testRelation1",
+    "properties": {
+      "keytype": "fk",
+      "relation": "one-to-one",
+      "typevalue": "id:id"
+    },
+    "out": "$entity1ForRelation"
+  }
+]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>[
@@ -717,6 +736,7 @@
     "in": "$entity2ForRelation"
   }
 ]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>[
@@ -747,6 +767,11 @@
     "in": "$entity2ForRelation"
   }
 ]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-updateEntities-Test-4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>[
@@ -764,6 +789,7 @@
     "in": "$entity2ForRelation"
   }
 ]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>[
@@ -781,15 +807,39 @@
     "in": "$entity2ForRelation"
   }
 ]</t>
-  </si>
-  <si>
-    <t>not exists</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>101400</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>good request,update multiple relations,data received</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bad request, entity id not exist</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[
+  {
+    "id" : "1234",
+    "label" : "testEntity1",
+    "properties" : {
+      "metadata_node_type" : "entity"
+    }
+  }
+]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>good request,delete multiple relations</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>testRelation1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>testRelation2,testRelation3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -800,20 +850,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1197,11 +1247,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1CD2C6C-7513-4EBA-9D12-F75700A492B3}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.109375" style="14" bestFit="1" customWidth="1"/>
@@ -1213,7 +1263,7 @@
     <col min="8" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1236,7 +1286,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -1244,7 +1294,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>21</v>
+        <v>137</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>51</v>
@@ -1259,7 +1309,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
@@ -1270,17 +1320,17 @@
         <v>23</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>32</v>
       </c>
@@ -1291,38 +1341,38 @@
         <v>24</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>34</v>
       </c>
@@ -1333,17 +1383,17 @@
         <v>27</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>35</v>
       </c>
@@ -1366,7 +1416,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
@@ -1404,7 +1454,7 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -1415,7 +1465,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1435,9 +1485,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1453,15 +1503,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2">
         <v>200</v>
@@ -1473,15 +1523,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D4" s="2">
         <v>200</v>
@@ -1493,15 +1543,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" s="2">
         <v>200</v>
@@ -1524,11 +1574,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3E9BB9-23BC-452F-AE17-4472AC4F82DB}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.77734375" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.109375" style="18" bestFit="1" customWidth="1"/>
@@ -1542,7 +1592,7 @@
     <col min="10" max="16384" width="8.77734375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
@@ -1550,7 +1600,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>17</v>
@@ -1571,21 +1621,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="148.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="236.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="F2" s="11">
         <v>1234</v>
@@ -1600,19 +1650,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="148.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="231.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>79</v>
@@ -1627,9 +1677,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>10</v>
@@ -1650,9 +1700,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>11</v>
@@ -1688,7 +1738,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="14" bestFit="1" customWidth="1"/>
@@ -1701,7 +1751,7 @@
     <col min="9" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1727,7 +1777,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>37</v>
       </c>
@@ -1753,7 +1803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>40</v>
       </c>
@@ -1765,17 +1815,17 @@
         <v>45</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>46</v>
       </c>
@@ -1787,17 +1837,17 @@
         <v>43</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>47</v>
       </c>
@@ -1809,17 +1859,17 @@
         <v>44</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>48</v>
       </c>
@@ -1860,7 +1910,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="5" bestFit="1" customWidth="1"/>
@@ -1873,7 +1923,7 @@
     <col min="9" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1899,7 +1949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="138" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="132" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>56</v>
       </c>
@@ -1925,7 +1975,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
@@ -1944,10 +1994,10 @@
         <v>101400</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>58</v>
       </c>
@@ -1966,7 +2016,7 @@
         <v>101400</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1984,7 +2034,7 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -1995,7 +2045,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2015,7 +2065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>60</v>
       </c>
@@ -2033,7 +2083,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>61</v>
       </c>
@@ -2053,7 +2103,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>62</v>
       </c>
@@ -2073,7 +2123,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>63</v>
       </c>
@@ -2108,7 +2158,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
@@ -2119,7 +2169,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2139,7 +2189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>65</v>
       </c>
@@ -2159,7 +2209,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>66</v>
       </c>
@@ -2179,7 +2229,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
@@ -2205,10 +2255,10 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.109375" style="5" bestFit="1" customWidth="1"/>
@@ -2221,7 +2271,7 @@
     <col min="9" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -2247,7 +2297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>56</v>
       </c>
@@ -2273,7 +2323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="248.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
@@ -2299,7 +2349,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>58</v>
       </c>
@@ -2321,7 +2371,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>76</v>
       </c>
@@ -2355,10 +2405,10 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="5" bestFit="1" customWidth="1"/>
@@ -2371,7 +2421,7 @@
     <col min="9" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -2397,18 +2447,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E2" s="8">
         <v>200</v>
@@ -2423,126 +2473,126 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>134</v>
-      </c>
       <c r="F6" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>135</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E8" s="8">
         <v>400</v>
@@ -2555,16 +2605,16 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E9" s="8">
         <v>400</v>
@@ -2577,16 +2627,16 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E10" s="8">
         <v>200</v>
@@ -2612,11 +2662,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E404F4D5-3387-4965-A2C7-1B0564B984EB}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="14" bestFit="1" customWidth="1"/>
@@ -2630,7 +2680,7 @@
     <col min="10" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -2638,7 +2688,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>17</v>
@@ -2659,21 +2709,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F2" s="12">
         <v>200</v>
@@ -2688,19 +2738,19 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F3" s="12">
         <v>200</v>
@@ -2715,7 +2765,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>46</v>
       </c>
@@ -2728,40 +2778,40 @@
         <v>45</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="189" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="194.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>48</v>
       </c>
@@ -2771,13 +2821,13 @@
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12" t="s">
@@ -2799,7 +2849,7 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="14" bestFit="1" customWidth="1"/>
@@ -2813,7 +2863,7 @@
     <col min="10" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
@@ -2821,7 +2871,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>17</v>
@@ -2842,21 +2892,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="248.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F2" s="7">
         <v>1234</v>
@@ -2871,9 +2921,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>10</v>
@@ -2891,12 +2941,12 @@
         <v>101400</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>11</v>
@@ -2914,7 +2964,7 @@
         <v>101400</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete entitymanagement test case:duplicated additional properties
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3990DB7A-F45F-4CA3-A7C1-560DEDFC8F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B454F20D-3DCD-4DFD-AE81-42A4F044C92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="createEntities" sheetId="17" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="227">
   <si>
     <t>testEntity1</t>
   </si>
@@ -554,13 +554,6 @@
 duplicated label</t>
   </si>
   <si>
-    <t>bad request,create one entity,
-duplicated additional properties</t>
-  </si>
-  <si>
-    <t>DUPLICATED_ADDITIONAL_PROPERTIES</t>
-  </si>
-  <si>
     <t>ILLEGAL_PROPERTY_KEY</t>
   </si>
   <si>
@@ -618,9 +611,6 @@
         }
     }
 ]</t>
-  </si>
-  <si>
-    <t>snc-entityMgmt-createEntities-Test-20</t>
   </si>
   <si>
     <t>good request,update one entity,
@@ -756,20 +746,6 @@
             "metadata_node_pk": "id",
             "id": "String",
             "name": "String"
-        }
-    }
-]</t>
-  </si>
-  <si>
-    <t>[
-    {
-        "id": "1234",
-        "label": "testEntity4",
-        "properties": {
-            "metadata_node_type": "entity",
-            "metadata_node_pk": "id",
-            "id": "String",
-            "id": "String"
         }
     }
 ]</t>
@@ -1931,11 +1907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858AADA8-A0C1-44F7-925E-7419FEAFD599}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2302,7 +2278,7 @@
         <v>125</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D15" s="12">
         <v>400</v>
@@ -2324,10 +2300,10 @@
         <v>120</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D16" s="12">
         <v>400</v>
@@ -2341,7 +2317,7 @@
       <c r="G16" s="12"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2349,10 +2325,10 @@
         <v>121</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D17" s="12">
         <v>400</v>
@@ -2366,7 +2342,7 @@
       <c r="G17" s="12"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2374,10 +2350,10 @@
         <v>122</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D18" s="12">
         <v>400</v>
@@ -2391,7 +2367,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2399,10 +2375,10 @@
         <v>123</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>140</v>
       </c>
       <c r="D19" s="12">
         <v>400</v>
@@ -2424,50 +2400,25 @@
         <v>124</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>135</v>
+        <v>54</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" s="12">
-        <v>400</v>
-      </c>
-      <c r="E20" s="12">
-        <v>101400</v>
+        <v>145</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G20" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="H20" s="6"/>
-      <c r="I20" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="I20" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2561,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D4" s="2">
         <v>200</v>
@@ -2604,8 +2555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3E9BB9-23BC-452F-AE17-4472AC4F82DB}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2659,10 +2610,10 @@
         <v>82</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>71</v>
@@ -2689,10 +2640,10 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>58</v>
@@ -2727,7 +2678,7 @@
         <v>86</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
@@ -2741,7 +2692,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="10"/>
       <c r="F5" s="16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G5" s="10">
         <v>200</v>
@@ -2820,13 +2771,13 @@
         <v>26</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E2" s="12">
         <v>200</v>
@@ -2874,7 +2825,7 @@
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>85</v>
@@ -2888,7 +2839,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2900,7 +2851,7 @@
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>85</v>
@@ -2909,7 +2860,7 @@
         <v>86</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="6"/>
@@ -2920,13 +2871,13 @@
         <v>32</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E6" s="12">
         <v>200</v>
@@ -3042,7 +2993,7 @@
         <v>101400</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -3064,7 +3015,7 @@
         <v>101400</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3159,7 +3110,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D4" s="2">
         <v>200</v>
@@ -3359,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F2" s="10">
         <v>200</v>
@@ -3379,7 +3330,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>57</v>
@@ -3416,7 +3367,7 @@
         <v>86</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -3429,7 +3380,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F5" s="10">
         <v>200</v>
@@ -3509,13 +3460,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E2" s="8">
         <v>200</v>
@@ -3537,11 +3488,11 @@
         <v>60</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E3" s="8">
         <v>400</v>
@@ -3559,11 +3510,11 @@
         <v>61</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E4" s="8">
         <v>400</v>
@@ -3581,11 +3532,11 @@
         <v>62</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E5" s="8">
         <v>400</v>
@@ -3603,11 +3554,11 @@
         <v>63</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E6" s="8">
         <v>400</v>
@@ -3625,11 +3576,11 @@
         <v>64</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E7" s="8">
         <v>400</v>
@@ -3647,11 +3598,11 @@
         <v>65</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E8" s="8">
         <v>400</v>
@@ -3665,7 +3616,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
@@ -3673,11 +3624,11 @@
         <v>66</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E9" s="8">
         <v>400</v>
@@ -3686,7 +3637,7 @@
         <v>101400</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="6"/>
@@ -3697,11 +3648,11 @@
         <v>67</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E10" s="8">
         <v>400</v>
@@ -3715,19 +3666,19 @@
       <c r="H10" s="12"/>
       <c r="I10" s="6"/>
       <c r="J10" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E11" s="8">
         <v>400</v>
@@ -3736,7 +3687,7 @@
         <v>101400</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="6"/>
@@ -3744,14 +3695,14 @@
     </row>
     <row r="12" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E12" s="8">
         <v>400</v>
@@ -3770,14 +3721,14 @@
     </row>
     <row r="13" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E13" s="8">
         <v>400</v>
@@ -3796,14 +3747,14 @@
     </row>
     <row r="14" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E14" s="8">
         <v>400</v>
@@ -3817,19 +3768,19 @@
       <c r="H14" s="12"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>167</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E15" s="8">
         <v>400</v>
@@ -3848,14 +3799,14 @@
     </row>
     <row r="16" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E16" s="8">
         <v>400</v>
@@ -3874,14 +3825,14 @@
     </row>
     <row r="17" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E17" s="8">
         <v>400</v>
@@ -3900,14 +3851,14 @@
     </row>
     <row r="18" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E18" s="8">
         <v>400</v>
@@ -3926,14 +3877,14 @@
     </row>
     <row r="19" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E19" s="8">
         <v>400</v>
@@ -3952,14 +3903,14 @@
     </row>
     <row r="20" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E20" s="8">
         <v>400</v>
@@ -3978,14 +3929,14 @@
     </row>
     <row r="21" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E21" s="8">
         <v>400</v>
@@ -4004,14 +3955,14 @@
     </row>
     <row r="22" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E22" s="8">
         <v>400</v>
@@ -4030,14 +3981,14 @@
     </row>
     <row r="23" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E23" s="8">
         <v>400</v>
@@ -4056,14 +4007,14 @@
     </row>
     <row r="24" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E24" s="8">
         <v>400</v>
@@ -4077,19 +4028,19 @@
       <c r="H24" s="12"/>
       <c r="I24" s="6"/>
       <c r="J24" s="7" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E25" s="8">
         <v>200</v>
@@ -4101,7 +4052,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="7"/>
@@ -4177,16 +4128,16 @@
         <v>26</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F2" s="12">
         <v>200</v>
@@ -4231,12 +4182,12 @@
         <v>30</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>85</v>
@@ -4250,7 +4201,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4258,12 +4209,12 @@
         <v>31</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>85</v>
@@ -4272,7 +4223,7 @@
         <v>86</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="6"/>
@@ -4287,10 +4238,10 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F6" s="12">
         <v>200</v>
@@ -4373,10 +4324,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>71</v>
@@ -4414,7 +4365,7 @@
         <v>101400</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
@@ -4437,7 +4388,7 @@
         <v>101400</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify entitymanagement test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B454F20D-3DCD-4DFD-AE81-42A4F044C92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF23B3F-F982-4D14-B1FA-4195FC406DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="createEntities" sheetId="17" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="230">
   <si>
     <t>testEntity1</t>
   </si>
@@ -314,14 +314,6 @@
 ]</t>
   </si>
   <si>
-    <t>bad request,create one entity,
-id is null</t>
-  </si>
-  <si>
-    <t>bad request,create one entity,
-properties is null</t>
-  </si>
-  <si>
     <t>[
     {
         "id": "1234",
@@ -545,9 +537,6 @@
   <si>
     <t>bad request,create one entity,
 no additional properties</t>
-  </si>
-  <si>
-    <t>NO_ADDITIONAL_PROPERTIES</t>
   </si>
   <si>
     <t>bad request,create one entity,
@@ -848,14 +837,6 @@
   </si>
   <si>
     <t>bad request,create one relation,
-out is not exists</t>
-  </si>
-  <si>
-    <t>bad request,create one relation,
-in is not exist</t>
-  </si>
-  <si>
-    <t>bad request,create one relation,
 label is illegal</t>
   </si>
   <si>
@@ -1158,10 +1139,6 @@
   <si>
     <t>bad request,create one relation,
 properties-typevalue is null</t>
-  </si>
-  <si>
-    <t>bad request,create one relation,
-properties-typevalue is not exist in entity of out/in</t>
   </si>
   <si>
     <t>[
@@ -1496,6 +1473,41 @@
   </si>
   <si>
     <t>testRelation2,testRelation3</t>
+  </si>
+  <si>
+    <t>bad request,create one entity,
+absence of id</t>
+  </si>
+  <si>
+    <t>bad request,create one entity,
+absence of label</t>
+  </si>
+  <si>
+    <t>bad request,create one entity,
+absence of properties</t>
+  </si>
+  <si>
+    <t>bad request,create one entity,
+absence of metadata_node_type</t>
+  </si>
+  <si>
+    <t>bad request,create one entity,
+absence of metadata_node_pk</t>
+  </si>
+  <si>
+    <t>NO_ADDITIONAL_PROPERTIES,ILLEGAL_PROPERTY_VALUE</t>
+  </si>
+  <si>
+    <t>bad request,create one relation,
+out value is not exists</t>
+  </si>
+  <si>
+    <t>bad request,create one relation,
+in value is not exist</t>
+  </si>
+  <si>
+    <t>bad request,create one relation,
+properties-type value is not exist in entity of out/in</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1622,9 +1634,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1909,22 +1918,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858AADA8-A0C1-44F7-925E-7419FEAFD599}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
@@ -1951,10 +1960,10 @@
         <v>33</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1962,7 +1971,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>87</v>
@@ -1987,10 +1996,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>88</v>
+        <v>221</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>85</v>
@@ -2008,10 +2017,10 @@
         <v>21</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>18</v>
+        <v>222</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>85</v>
@@ -2029,10 +2038,10 @@
         <v>22</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>89</v>
+        <v>223</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>85</v>
@@ -2050,10 +2059,10 @@
         <v>23</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" s="12">
         <v>400</v>
@@ -2062,12 +2071,12 @@
         <v>101400</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2078,7 +2087,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D7" s="12">
         <v>400</v>
@@ -2087,12 +2096,12 @@
         <v>101400</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2100,7 +2109,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>87</v>
@@ -2112,23 +2121,23 @@
         <v>101400</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>17</v>
+        <v>224</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D9" s="12">
         <v>400</v>
@@ -2137,23 +2146,23 @@
         <v>101400</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>108</v>
+        <v>225</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="12">
         <v>400</v>
@@ -2162,23 +2171,23 @@
         <v>101400</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" s="12">
         <v>400</v>
@@ -2187,23 +2196,23 @@
         <v>101400</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D12" s="12">
         <v>400</v>
@@ -2212,23 +2221,23 @@
         <v>101400</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D13" s="12">
         <v>400</v>
@@ -2237,23 +2246,23 @@
         <v>101400</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D14" s="12">
         <v>400</v>
@@ -2262,23 +2271,23 @@
         <v>101400</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D15" s="12">
         <v>400</v>
@@ -2287,23 +2296,23 @@
         <v>101400</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="6" t="s">
-        <v>126</v>
+      <c r="I15" s="7" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D16" s="12">
         <v>400</v>
@@ -2312,23 +2321,23 @@
         <v>101400</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D17" s="12">
         <v>400</v>
@@ -2337,23 +2346,23 @@
         <v>101400</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D18" s="12">
         <v>400</v>
@@ -2362,23 +2371,23 @@
         <v>101400</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D19" s="12">
         <v>400</v>
@@ -2387,23 +2396,23 @@
         <v>101400</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>35</v>
@@ -2512,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D4" s="2">
         <v>200</v>
@@ -2610,10 +2619,10 @@
         <v>82</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>71</v>
@@ -2640,10 +2649,10 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>58</v>
@@ -2678,7 +2687,7 @@
         <v>86</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
@@ -2692,7 +2701,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="10"/>
       <c r="F5" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G5" s="10">
         <v>200</v>
@@ -2760,10 +2769,10 @@
         <v>33</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2771,13 +2780,13 @@
         <v>26</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E2" s="12">
         <v>200</v>
@@ -2825,7 +2834,7 @@
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>85</v>
@@ -2834,12 +2843,12 @@
         <v>86</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2851,7 +2860,7 @@
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>85</v>
@@ -2860,7 +2869,7 @@
         <v>86</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="6"/>
@@ -2871,13 +2880,13 @@
         <v>32</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E6" s="12">
         <v>200</v>
@@ -2993,7 +3002,7 @@
         <v>101400</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -3015,7 +3024,7 @@
         <v>101400</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3110,7 +3119,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D4" s="2">
         <v>200</v>
@@ -3310,7 +3319,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F2" s="10">
         <v>200</v>
@@ -3330,7 +3339,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>57</v>
@@ -3367,7 +3376,7 @@
         <v>86</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -3380,7 +3389,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F5" s="10">
         <v>200</v>
@@ -3403,9 +3412,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D926784-FA98-439E-A0B5-45972E5852A3}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -3449,10 +3458,10 @@
         <v>33</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
@@ -3460,13 +3469,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E2" s="8">
         <v>200</v>
@@ -3488,11 +3497,11 @@
         <v>60</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E3" s="8">
         <v>400</v>
@@ -3510,11 +3519,11 @@
         <v>61</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E4" s="8">
         <v>400</v>
@@ -3532,11 +3541,11 @@
         <v>62</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E5" s="8">
         <v>400</v>
@@ -3554,11 +3563,11 @@
         <v>63</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E6" s="8">
         <v>400</v>
@@ -3576,11 +3585,11 @@
         <v>64</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E7" s="8">
         <v>400</v>
@@ -3598,11 +3607,11 @@
         <v>65</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>156</v>
+        <v>227</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E8" s="8">
         <v>400</v>
@@ -3611,12 +3620,12 @@
         <v>101400</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="6"/>
       <c r="J8" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
@@ -3624,11 +3633,11 @@
         <v>66</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E9" s="8">
         <v>400</v>
@@ -3636,23 +3645,25 @@
       <c r="F9" s="8">
         <v>101400</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>144</v>
+      <c r="G9" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
+      <c r="J9" s="7" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E10" s="8">
         <v>400</v>
@@ -3661,24 +3672,24 @@
         <v>101400</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="6"/>
       <c r="J10" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E11" s="8">
         <v>400</v>
@@ -3686,23 +3697,25 @@
       <c r="F11" s="8">
         <v>101400</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>144</v>
+      <c r="G11" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="7" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E12" s="8">
         <v>400</v>
@@ -3711,24 +3724,24 @@
         <v>101400</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="6"/>
       <c r="J12" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E13" s="8">
         <v>400</v>
@@ -3737,24 +3750,24 @@
         <v>101400</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="6"/>
       <c r="J13" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E14" s="8">
         <v>400</v>
@@ -3763,24 +3776,24 @@
         <v>101400</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E15" s="8">
         <v>400</v>
@@ -3789,24 +3802,24 @@
         <v>101400</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="6"/>
       <c r="J15" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E16" s="8">
         <v>400</v>
@@ -3815,24 +3828,24 @@
         <v>101400</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="6"/>
       <c r="J16" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E17" s="8">
         <v>400</v>
@@ -3841,24 +3854,24 @@
         <v>101400</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="6"/>
       <c r="J17" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E18" s="8">
         <v>400</v>
@@ -3867,24 +3880,24 @@
         <v>101400</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="6"/>
       <c r="J18" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E19" s="8">
         <v>400</v>
@@ -3893,24 +3906,24 @@
         <v>101400</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="6"/>
       <c r="J19" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E20" s="8">
         <v>400</v>
@@ -3919,24 +3932,24 @@
         <v>101400</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="6"/>
       <c r="J20" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E21" s="8">
         <v>400</v>
@@ -3945,24 +3958,24 @@
         <v>101400</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="6"/>
       <c r="J21" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E22" s="8">
         <v>400</v>
@@ -3971,24 +3984,24 @@
         <v>101400</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="6"/>
       <c r="J22" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E23" s="8">
         <v>400</v>
@@ -3997,24 +4010,24 @@
         <v>101400</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="6"/>
       <c r="J23" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>196</v>
+        <v>229</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E24" s="8">
         <v>400</v>
@@ -4023,24 +4036,24 @@
         <v>101400</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="6"/>
       <c r="J24" s="7" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E25" s="8">
         <v>200</v>
@@ -4052,7 +4065,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="7"/>
@@ -4117,10 +4130,10 @@
         <v>33</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4128,16 +4141,16 @@
         <v>26</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F2" s="12">
         <v>200</v>
@@ -4182,12 +4195,12 @@
         <v>30</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>85</v>
@@ -4196,12 +4209,12 @@
         <v>86</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4209,12 +4222,12 @@
         <v>31</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>85</v>
@@ -4223,7 +4236,7 @@
         <v>86</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="6"/>
@@ -4238,10 +4251,10 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F6" s="12">
         <v>200</v>
@@ -4324,10 +4337,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>71</v>
@@ -4365,7 +4378,7 @@
         <v>101400</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
@@ -4388,7 +4401,7 @@
         <v>101400</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add publish check cases
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
@@ -5,25 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F72666-426E-4DD7-9FF2-F33CF3F98520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF0AA9B-C9C8-4598-B255-CE316C47DB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="createEntities" sheetId="17" r:id="rId1"/>
-    <sheet name="updateEntities" sheetId="18" r:id="rId2"/>
-    <sheet name="getEntityById" sheetId="2" r:id="rId3"/>
-    <sheet name="getEntities" sheetId="12" r:id="rId4"/>
-    <sheet name="getEntitiesLabelLike" sheetId="14" r:id="rId5"/>
-    <sheet name="deleteEntities" sheetId="4" r:id="rId6"/>
-    <sheet name="createRelations" sheetId="19" r:id="rId7"/>
-    <sheet name="updateRelations" sheetId="20" r:id="rId8"/>
-    <sheet name="getRelationById" sheetId="7" r:id="rId9"/>
-    <sheet name="getRelations" sheetId="6" r:id="rId10"/>
-    <sheet name="deleteRelations" sheetId="16" r:id="rId11"/>
+    <sheet name="publishCheck" sheetId="21" r:id="rId1"/>
+    <sheet name="createEntities" sheetId="17" r:id="rId2"/>
+    <sheet name="updateEntities" sheetId="18" r:id="rId3"/>
+    <sheet name="getEntityById" sheetId="2" r:id="rId4"/>
+    <sheet name="getEntities" sheetId="12" r:id="rId5"/>
+    <sheet name="getEntitiesLabelLike" sheetId="14" r:id="rId6"/>
+    <sheet name="deleteEntities" sheetId="4" r:id="rId7"/>
+    <sheet name="createRelations" sheetId="19" r:id="rId8"/>
+    <sheet name="updateRelations" sheetId="20" r:id="rId9"/>
+    <sheet name="getRelationById" sheetId="7" r:id="rId10"/>
+    <sheet name="getRelations" sheetId="6" r:id="rId11"/>
+    <sheet name="deleteRelations" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="323">
   <si>
     <t>testEntity1</t>
   </si>
@@ -1509,30 +1510,1359 @@
     <t>bad request,create one relation,
 properties-type value is not exist in entity of out/in</t>
   </si>
+  <si>
+    <t>warningRule</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>erroRule</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-1</t>
+  </si>
+  <si>
+    <t>good request, No error</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bad request, No metadata_node_type field</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "pc_test1",
+				"properties": {
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "pc_test2",
+				"properties": {
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "pc_edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABSENT_OF_PROPERTY_KEY</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-2-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bad request, No metadata_node_pk field</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "pc_test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "pc_test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "pc_edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-3</t>
+  </si>
+  <si>
+    <t>bad request, illegal entity label with chinese and special character</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "中文",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "~!@#$%^&amp;*()_+=",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ILLEGAL_LABEL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-4</t>
+  </si>
+  <si>
+    <t>good request, No error  with legal entity label with enlish and number and underline</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "_name123",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "NAME_1234567890",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad request, duplicated entity label </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DUPLICATED_LABEL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-6</t>
+  </si>
+  <si>
+    <t>good request, NO error  with same entity label in upper case</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "TEST1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-7</t>
+  </si>
+  <si>
+    <t>bad request,illegal entity properity key with chinese character</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "pc_test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"中文": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "pc_test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "pc_edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-8</t>
+  </si>
+  <si>
+    <t>good request, No error with legal entity properity key</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"_name1234567890": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"NAME_1234567890": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-9</t>
+  </si>
+  <si>
+    <t>good request, No error with legal entity properity value in Integer|String|Double|Float|Boolean|Long|Short|Byte|Char|LocalDateTime</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "Integer",
+					"score1": "Double",
+					"score2": "Float",
+					"score3": "Char"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "Boolean",
+					"id": "Long",
+					"score1": "Short",
+					"score2": "Byte",
+					"score3": "LocalDateTime"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-10</t>
+  </si>
+  <si>
+    <t>bad request, illegal entity properity value in SMALLINT|REAL|BINARY|BIT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "SMALLINT",
+					"id": "REAL"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "BINARY",
+					"id": "BIT"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ILLEGAL_PROPERTY_VALUE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-11</t>
+  </si>
+  <si>
+    <t>bad request,Relation in value is NOT exist in entity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "4",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+				"keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENTITY_NOT_EXIST_ON_RELATION</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-12</t>
+  </si>
+  <si>
+    <t>bad request, Relation out value is NOT exist in entity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "4",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-17</t>
+  </si>
+  <si>
+    <t>bad request, Relation without relation field</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-18</t>
+  </si>
+  <si>
+    <t>good request, No error with legal relation value of one-to-many</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-many",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-19</t>
+  </si>
+  <si>
+    <t>good request, No error with legal relation value of many-to-one</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "many-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-20</t>
+  </si>
+  <si>
+    <t>bad request, Illegal relation value of many-to-many</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "many-to-many",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-21</t>
+  </si>
+  <si>
+    <t>bad request, No keytype field</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-22</t>
+  </si>
+  <si>
+    <t>bad request, Illegal keytype value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "test",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-23</t>
+  </si>
+  <si>
+    <t>bad request, two edges between two entities</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		},
+{
+			"id":"4",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DUPLICATED_EDGES_BETWEEN_VERTICES</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-24</t>
+  </si>
+  <si>
+    <t>bad request, typevalue": "id:id1"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id1",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RELATION_FIELD_NOT_EXIST_ON_ENTITY</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-25</t>
+  </si>
+  <si>
+    <t>bad request, typevalue": "id1:id"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id1:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-26</t>
+  </si>
+  <si>
+    <t>bad request, NO_ADDITIONAL_PROPERTIES in entity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "pc_test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id"
+				}
+			},
+			{
+				"id": "2",
+				"label": "pc_test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "pc_edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO_ADDITIONAL_PROPERTIES</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-27</t>
+  </si>
+  <si>
+    <t>bad request, NO_ADDITIONAL_PROPERTIES in relation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "pc_test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "pc_test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "pc_edge",
+			"out": "2",
+			"properties": {
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO_ADDITIONAL_PROPERTIES</t>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good request, instance node type </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "pc_test1",
+				"properties": {
+					"metadata_node_type": "instance",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "pc_test2",
+				"properties": {
+					"metadata_node_type": "instance",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "pc_edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-29</t>
+  </si>
+  <si>
+    <t>good request, entity multiple metadata_mode_pk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "pc_test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id,name",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "pc_test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id,name",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "pc_edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-30</t>
+  </si>
+  <si>
+    <t>good request, relation multiple typevalue</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "pc_test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "pc_test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "pc_edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id,name:name",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"create": {
+		"entities": [{
+				"id": "1",
+				"label": "pc_test1",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			},
+			{
+				"id": "2",
+				"label": "pc_test2",
+				"properties": {
+					"metadata_node_type": "entity",
+					"metadata_node_pk": "id",
+					"name": "String",
+					"id": "String"
+				}
+			}
+		],
+		"relations": [{
+			"id": "3",
+			"in": "1",
+			"label": "pc_edge",
+			"out": "2",
+			"properties": {
+			    "keytype": "fk",
+				"relation": "one-to-one",
+				"typevalue": "id:id",
+				"additionalProp3": "String"
+			}
+		}]
+	}
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1583,7 +2913,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1635,6 +2965,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1915,15 +3248,1100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E1FA72-6F3A-4DD5-9877-D14B2446AEF5}">
+  <dimension ref="U1:AB28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="21" max="21" width="60.5546875" customWidth="1"/>
+    <col min="22" max="22" width="48.21875" customWidth="1"/>
+    <col min="23" max="23" width="87.88671875" customWidth="1"/>
+    <col min="28" max="28" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="21:28" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="U1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U2" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="5"/>
+    </row>
+    <row r="3" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U3" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="X3" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U4" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="V4" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="W4" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="X4" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U5" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="V5" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="W5" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="X5" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U6" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="V6" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="W6" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="X6" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+    </row>
+    <row r="7" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U7" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="V7" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="W7" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="X7" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U8" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="V8" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="W8" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="X8" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+    </row>
+    <row r="9" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U9" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="V9" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="W9" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="X9" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U10" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="V10" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="W10" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="X10" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+    </row>
+    <row r="11" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U11" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="V11" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="W11" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="X11" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z11" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+    </row>
+    <row r="12" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U12" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="V12" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="W12" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="X12" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y12" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U13" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="V13" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="W13" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="X13" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U14" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="V14" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="W14" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="X14" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y14" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z14" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U15" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="V15" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="W15" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="X15" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y15" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z15" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U16" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="V16" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="W16" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="X16" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+    </row>
+    <row r="17" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U17" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="V17" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="W17" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="X17" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y17" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z17" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+    </row>
+    <row r="18" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U18" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="V18" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="W18" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="X18" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y18" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z18" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U19" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="V19" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="W19" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="X19" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y19" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z19" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U20" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="V20" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="W20" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="X20" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y20" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z20" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U21" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="V21" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="W21" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="X21" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y21" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z21" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U22" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="V22" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="W22" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="X22" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y22" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z22" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U23" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="V23" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="W23" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="X23" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y23" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z23" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U24" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="V24" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="W24" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="X24" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y24" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z24" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB24" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U25" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="V25" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="W25" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="X25" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y25" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z25" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="26" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U26" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="V26" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="W26" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="X26" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y26" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z26" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U27" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="V27" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="W27" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="X27" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y27" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z27" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U28" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="V28" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="W28" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="X28" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y28" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z28" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8CB3E4-B830-482F-A87D-FE5107D53FAD}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="316.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1234</v>
+      </c>
+      <c r="G2" s="12">
+        <v>200</v>
+      </c>
+      <c r="H2" s="12">
+        <v>100000</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6">
+        <v>400</v>
+      </c>
+      <c r="H3" s="6">
+        <v>101400</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="15">
+        <v>999999</v>
+      </c>
+      <c r="G4" s="6">
+        <v>400</v>
+      </c>
+      <c r="H4" s="6">
+        <v>101400</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7825D-C3D3-4455-B765-0D831E376750}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
+        <v>200</v>
+      </c>
+      <c r="E2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="2">
+        <v>200</v>
+      </c>
+      <c r="E3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="2">
+        <v>200</v>
+      </c>
+      <c r="E4" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="2">
+        <v>200</v>
+      </c>
+      <c r="E5" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3E9BB9-23BC-452F-AE17-4472AC4F82DB}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="148.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1234</v>
+      </c>
+      <c r="G2" s="12">
+        <v>200</v>
+      </c>
+      <c r="H2" s="12">
+        <v>100000</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="148.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="12">
+        <v>200</v>
+      </c>
+      <c r="H3" s="12">
+        <v>100000</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="10">
+        <v>400</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="10">
+        <v>200</v>
+      </c>
+      <c r="H5" s="10">
+        <v>100000</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858AADA8-A0C1-44F7-925E-7419FEAFD599}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.44140625" style="14" bestFit="1" customWidth="1"/>
@@ -1937,7 +4355,7 @@
     <col min="10" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1966,7 +4384,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
@@ -1991,7 +4409,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
@@ -2012,7 +4430,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -2033,7 +4451,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
@@ -2054,7 +4472,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
@@ -2079,7 +4497,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>24</v>
       </c>
@@ -2104,7 +4522,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -2129,7 +4547,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>91</v>
       </c>
@@ -2154,7 +4572,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>92</v>
       </c>
@@ -2179,7 +4597,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>93</v>
       </c>
@@ -2204,7 +4622,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>110</v>
       </c>
@@ -2229,7 +4647,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>111</v>
       </c>
@@ -2254,7 +4672,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>112</v>
       </c>
@@ -2279,7 +4697,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>117</v>
       </c>
@@ -2304,7 +4722,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>118</v>
       </c>
@@ -2329,7 +4747,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>119</v>
       </c>
@@ -2354,7 +4772,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>120</v>
       </c>
@@ -2379,7 +4797,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>121</v>
       </c>
@@ -2404,7 +4822,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>122</v>
       </c>
@@ -2436,291 +4854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7825D-C3D3-4455-B765-0D831E376750}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2">
-        <v>200</v>
-      </c>
-      <c r="E2" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="2">
-        <v>200</v>
-      </c>
-      <c r="E3" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D4" s="2">
-        <v>200</v>
-      </c>
-      <c r="E4" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="2">
-        <v>200</v>
-      </c>
-      <c r="E5" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3E9BB9-23BC-452F-AE17-4472AC4F82DB}">
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="30.77734375" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="17"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="148.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="11">
-        <v>1234</v>
-      </c>
-      <c r="G2" s="12">
-        <v>200</v>
-      </c>
-      <c r="H2" s="12">
-        <v>100000</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="148.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="12">
-        <v>200</v>
-      </c>
-      <c r="H3" s="12">
-        <v>100000</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="69" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="10">
-        <v>400</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="10">
-        <v>200</v>
-      </c>
-      <c r="H5" s="10">
-        <v>100000</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B97966-D445-41D3-A12C-5E1768A05176}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -2728,7 +4862,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="14" bestFit="1" customWidth="1"/>
@@ -2743,7 +4877,7 @@
     <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -2775,7 +4909,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>26</v>
       </c>
@@ -2803,7 +4937,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>27</v>
       </c>
@@ -2825,7 +4959,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>30</v>
       </c>
@@ -2851,7 +4985,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>31</v>
       </c>
@@ -2875,7 +5009,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -2910,7 +5044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68ECACFD-75AA-40A8-8500-FACA5E36F33B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -2918,7 +5052,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="5" bestFit="1" customWidth="1"/>
@@ -2931,7 +5065,7 @@
     <col min="9" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -2957,7 +5091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>38</v>
       </c>
@@ -2983,7 +5117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="69" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>39</v>
       </c>
@@ -3005,7 +5139,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>40</v>
       </c>
@@ -3034,7 +5168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F02205-0A11-4FA8-921F-0678D65FEEFD}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -3042,7 +5176,7 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -3053,7 +5187,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -3073,7 +5207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>41</v>
       </c>
@@ -3091,7 +5225,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
@@ -3111,7 +5245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
@@ -3131,7 +5265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>44</v>
       </c>
@@ -3158,7 +5292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98D4ADA-9D8A-46CB-9E8C-40F98F5CFA96}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -3166,7 +5300,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
@@ -3177,7 +5311,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -3197,7 +5331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
@@ -3217,7 +5351,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -3237,7 +5371,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
@@ -3258,7 +5392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C10F18-6774-4DA2-A97E-6CA070C2B102}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -3266,7 +5400,7 @@
       <selection activeCell="F5" sqref="F5:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.109375" style="5" bestFit="1" customWidth="1"/>
@@ -3279,7 +5413,7 @@
     <col min="9" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -3305,7 +5439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="158.4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>38</v>
       </c>
@@ -3331,7 +5465,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="303.60000000000002" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>39</v>
       </c>
@@ -3357,7 +5491,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="69" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>40</v>
       </c>
@@ -3379,7 +5513,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>55</v>
       </c>
@@ -3408,7 +5542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D926784-FA98-439E-A0B5-45972E5852A3}">
   <dimension ref="A1:J25"/>
   <sheetViews>
@@ -3417,7 +5551,7 @@
       <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.109375" style="5" bestFit="1" customWidth="1"/>
@@ -3432,7 +5566,7 @@
     <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -3464,7 +5598,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -3492,7 +5626,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
@@ -3514,7 +5648,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>61</v>
       </c>
@@ -3536,7 +5670,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>62</v>
       </c>
@@ -3558,7 +5692,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>63</v>
       </c>
@@ -3580,7 +5714,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>64</v>
       </c>
@@ -3602,7 +5736,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>65</v>
       </c>
@@ -3628,7 +5762,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
@@ -3654,7 +5788,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>67</v>
       </c>
@@ -3680,7 +5814,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>154</v>
       </c>
@@ -3706,7 +5840,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>155</v>
       </c>
@@ -3732,7 +5866,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>156</v>
       </c>
@@ -3758,7 +5892,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>157</v>
       </c>
@@ -3784,7 +5918,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>158</v>
       </c>
@@ -3810,7 +5944,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>174</v>
       </c>
@@ -3836,7 +5970,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>175</v>
       </c>
@@ -3862,7 +5996,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>184</v>
       </c>
@@ -3888,7 +6022,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>185</v>
       </c>
@@ -3914,7 +6048,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>186</v>
       </c>
@@ -3940,7 +6074,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>187</v>
       </c>
@@ -3966,7 +6100,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>188</v>
       </c>
@@ -3992,7 +6126,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>192</v>
       </c>
@@ -4018,7 +6152,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>201</v>
       </c>
@@ -4044,7 +6178,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>208</v>
       </c>
@@ -4077,7 +6211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F5FE0E-8788-403D-8502-6CD26A71119B}">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -4085,7 +6219,7 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.77734375" style="14" bestFit="1" customWidth="1"/>
@@ -4101,7 +6235,7 @@
     <col min="12" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -4136,7 +6270,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>26</v>
       </c>
@@ -4167,7 +6301,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>27</v>
       </c>
@@ -4190,7 +6324,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>30</v>
       </c>
@@ -4217,7 +6351,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>31</v>
       </c>
@@ -4242,7 +6376,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -4276,137 +6410,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8CB3E4-B830-482F-A87D-FE5107D53FAD}">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="32" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="303.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1234</v>
-      </c>
-      <c r="G2" s="12">
-        <v>200</v>
-      </c>
-      <c r="H2" s="12">
-        <v>100000</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="69" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="6">
-        <v>400</v>
-      </c>
-      <c r="H3" s="6">
-        <v>101400</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="15">
-        <v>999999</v>
-      </c>
-      <c r="G4" s="6">
-        <v>400</v>
-      </c>
-      <c r="H4" s="6">
-        <v>101400</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add test case of sdl-7266
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-entity-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66450CF7-D010-45A0-98F5-7D628DB401C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36833100-D0AB-4D7A-836E-9E7248E7E691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" tabRatio="800" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" tabRatio="800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publishCheck" sheetId="21" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="402">
   <si>
     <t>testEntity1</t>
   </si>
@@ -3875,6 +3875,116 @@
   <si>
     <t>Edge [[abcde123]] not exist!</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-31</t>
+  </si>
+  <si>
+    <t>snc-entityMgmt-publishCheck-create-Test-32</t>
+  </si>
+  <si>
+    <t>{
+    "create": {
+        "entities": [
+            {
+                "id": "1",
+                "label": "pc_test1",
+                "properties": {
+                    "metadata_node_type": "entity",
+                    "metadata_node_pk": "id",
+                    "name": "String",
+                    "id": "String"
+                }
+            },
+            {
+                "id": "2",
+                "label": "pc_test2",
+                "properties": {
+                    "metadata_node_type": "entity",
+                    "metadata_node_pk": "id",
+                    "name": "String",
+                    "id": "String"
+                }
+            }
+        ],
+        "relations": [
+            {
+                "id": "3",
+                "in": "1",
+                "label": "pc_edge",
+                "out": "2",
+                "properties": {
+                    "keytype": "fk",
+                    "relation": "one-to-one",
+                    "typevalue": "id:id",
+                    "additionalProp3": "String",
+					"pc_edge":"String"
+                }
+            }
+        ]
+    }
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ILLEGAL_PROPERTY_KEY</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bad request, Graph cannot be import when edge label same with relation name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bad request, Graph cannot be import when edge label same with entity name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "create": {
+        "entities": [
+            {
+                "id": "1",
+                "label": "pc_test1",
+                "properties": {
+                    "metadata_node_type": "entity",
+                    "metadata_node_pk": "id",
+                    "name": "String",
+                    "id": "String"
+                }
+            },
+            {
+                "id": "2",
+                "label": "pc_test2",
+                "properties": {
+                    "metadata_node_type": "entity",
+                    "metadata_node_pk": "id",
+                    "name": "String",
+                    "id": "String",
+					"pc_edge":"String"
+                }
+            }
+        ],
+        "relations": [
+            {
+                "id": "3",
+                "in": "1",
+                "label": "pc_edge",
+                "out": "2",
+                "properties": {
+                    "keytype": "fk",
+                    "relation": "one-to-one",
+                    "typevalue": "id:id",
+                    "additionalProp3": "String"
+                }
+            }
+        ]
+    }
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4293,10 +4403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E1FA72-6F3A-4DD5-9877-D14B2446AEF5}">
-  <dimension ref="U1:AB28"/>
+  <dimension ref="U1:AB30"/>
   <sheetViews>
-    <sheetView topLeftCell="T5" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="W29" workbookViewId="0">
+      <selection activeCell="W30" sqref="W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4951,6 +5061,52 @@
       </c>
       <c r="Z28" s="5" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U29" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="V29" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="W29" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="X29" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y29" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z29" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="U30" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="V30" s="14" t="s">
+        <v>400</v>
+      </c>
+      <c r="W30" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="X30" s="5">
+        <v>200</v>
+      </c>
+      <c r="Y30" s="5">
+        <v>100000</v>
+      </c>
+      <c r="Z30" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -5633,7 +5789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F5FE0E-8788-403D-8502-6CD26A71119B}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>